<commit_message>
default filters; simple test
</commit_message>
<xml_diff>
--- a/examples/data/DiscussionAttendance.xlsx
+++ b/examples/data/DiscussionAttendance.xlsx
@@ -464,13 +464,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:E4"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -546,10 +546,6 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -560,10 +556,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -595,11 +591,6 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>